<commit_message>
UI Validations added V.73
</commit_message>
<xml_diff>
--- a/TestSuites/UploadExcel/TD_E2E.xlsx
+++ b/TestSuites/UploadExcel/TD_E2E.xlsx
@@ -223,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -389,7 +389,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -426,12 +425,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4923,8 +4916,8 @@
   </sheetPr>
   <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
@@ -5082,7 +5075,7 @@
           <t>P1</t>
         </is>
       </c>
-      <c r="E2" s="82" t="inlineStr">
+      <c r="E2" s="67" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
@@ -5102,9 +5095,9 @@
           <t>f4c16e81-bdcb-4795-9dce-3b36416eb748</t>
         </is>
       </c>
-      <c r="I2" s="83" t="inlineStr">
-        <is>
-          <t>24ef8838-956b-4808-9127-af8e42410826</t>
+      <c r="I2" s="68" t="inlineStr">
+        <is>
+          <t>24ef5959-677b-4808-9127-af8e42410423</t>
         </is>
       </c>
       <c r="L2" s="66" t="inlineStr">
@@ -5129,12 +5122,12 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>7273087</t>
-        </is>
-      </c>
-      <c r="Q2" s="81" t="inlineStr">
-        <is>
-          <t>3215545</t>
+          <t>7277770</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>3216069</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -5147,24 +5140,24 @@
           <t>CLOSED WITH ORDER</t>
         </is>
       </c>
-      <c r="T2" s="81" t="inlineStr">
+      <c r="T2" s="80" t="inlineStr">
         <is>
           <t>200</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7273087 for PriceProposal 24ef8838-956b-4808-9127-af8e42410826","version":"1.4.9-qa2.63","viaxPriceProposalId":"7273087","priceProposal":{"uid":"66fc0fad-e91d-483d-af93-e5c67154dfef","biId":"7273087","wAsRelatedOrder":null,"wAsSubmissionId":"24ef8838-956b-4808-9127-af8e42410826","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":"2026-04-01T15:05:17.269Z","wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-10-01T15:05:17.311Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef8838-956b-4808-9127-af8e42410826","edRefCode":"ACN3-2023-06-8838","articleDOI":"","journalId":"f4c16e81-bdcb-4795-9dce-3b36416eb748","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article","submissionDate":"2024-10-01","articleAcceptedDate":"2015-09-29","editorialStatus":"ACCEPTED","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"07030","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-10-01T15:05:18.212Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsAuthorFunds":null,"wAsPricing":{"isFunded":false,"availableWorkflowType":null,"woadInstitution":null,"prices":[{"basePrice":3850,"price":3850,"subtotal":3850,"tax":0,"total":3850,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef8838-956b-4808-9127-af8e42410826","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-8838","wAsSubmissionId":"24ef8838-956b-4808-9127-af8e42410826","wAsSubmissionDate":"2024-10-01","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"ACCEPTED","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article","ibrProduct":{"maId":"JDI","maName":"Journal of Diabetes Investigation","wAsJournalUuid":"f4c16e81-bdcb-4795-9dce-3b36416eb748","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20401124","wAsFlipDate":"2013-09-23","wAsJournalTitle":"Journal of Diabetes Investigation","wAsJournalGroupCode":"JDI","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"jdi@wiley.com"}}}]}}'}}}</t>
+          <t>{'data': {'testFunction': {'status': 200, 'data': '{"status":"SUCCESS","message":"Created Viax order 7277770 for PriceProposal 24ef5959-677b-4808-9127-af8e42410423","version":"1.4.9-qa2.67","viaxPriceProposalId":"7277770","priceProposal":{"uid":"67219d65-df52-4774-8edf-3582d7a8e9c8","biId":"7277770","wAsRelatedOrder":null,"wAsSubmissionId":"24ef5959-677b-4808-9127-af8e42410423","wAsReasonForReSendStatusChange":null,"wAsReasonForReOpenStatusChange":null,"wAsExpiryDateTime":"2026-04-30T02:43:49.819Z","wAsReopenDateTime":null,"bpStatus":{"code":"PriceDetermined"},"biCreatedAt":"2024-10-30T02:43:49.864Z","wAsPaymentType":"AuthorPaid","wAsPriceProposalPayload":{"requestId":"e5a1358c-2f36-4d12-8c68-fe0b8c46172a","submissionId":"24ef5959-677b-4808-9127-af8e42410423","edRefCode":"ACN3-2023-06-5959","articleDOI":"","journalId":"f4c16e81-bdcb-4795-9dce-3b36416eb748","sourceSystem":"EM","baseArticleType":"Research Article","displayArticleType":"Research Article","submissionDate":"2024-10-30","articleAcceptedDate":"2015-09-29","editorialStatus":"ACCEPTED","articleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","isManualOverrideRequired":false,"manualOverrideInstructions":"string","societyCodes":[],"promoCodes":[],"discountCodes":[],"authors":[{"role":"Corresponding Author","authorSequenceNumber":1,"firstName":"Jim","middleName":"M.","lastName":"TESSON","honorificPrefix":"Mr.","honorificSuffix":"","email":"TestAutomation@Wiley.com","affiliationIdType":"Ringgold","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"addressLocality":"Aix en Provence","countryCode":"US","country":"US","institution":"Grant Institute","department":"School of GeoSciences","stateProvince":"New Jersey","postalCode":"07030","streetAddress":["1832 Colvin Ave"]}]}]},"wAsOrderUniqueId":null,"wAsOrderStatus":null,"wAsLastEmailDate":null,"wAsSuppressEmail":false,"wAsDiscountCodes":[],"auAudit":{"updatedAt":{"dateTime":"2024-10-30T02:43:50.563Z"}},"wAsCountryCode":"US","wAsReferringJournal":null,"wAsReferringJournalRef":null,"wAsValidationErrors":[],"wAsPricing":{"isFunded":false,"woadInstitution":null,"prices":[{"basePrice":3850,"price":3850,"subtotal":3850,"tax":0,"total":3850,"discountAmount":0,"discountPercentage":0,"currencyCode":"USD","allDiscounts":[],"appliedDiscounts":[]}]},"wAsBillingDetails":[],"wAsManualDiscountAmount":null,"wAsManualOverrideRequired":false,"wAsManualDiscountPercentage":null,"wAsManualOverrideInstructions":"string","wAsManualOverrideAppliedTime":null,"wAsCorrespondingAuthor":{"orcId":null,"firstName":"Jim","lastName":"TESSON","email":"TestAutomation@Wiley.com","isResponsible":false,"affiliationIdType":"Ringgold","honorificPrefix":"Mr.","honorificSuffix":"","affiliations":[{"affiliationIds":[{"institutionId":"","institutionIdType":"Ringgold"}],"affiliationName":"Grant Institute","countryCode":"US","isPrimary":null}],"authorFunds":[]},"wAsResearchFunders":[],"attAttachments":[],"hiConsistsOf":[{"wAsEditorialDiscountCode":null,"biiSalable":{"maId":"24ef5959-677b-4808-9127-af8e42410423","wAsArticleId":null,"wAsArticleDoi":"","wAsArticleTitle":"Seismic slip history of the Pizzalto fault (Central Apennines Italy) using in situ-produced Clcosmic ray exposure dating and rare earth element concentrations.","wAsManuscriptId":"ACN3-2023-06-5959","wAsSubmissionId":"24ef5959-677b-4808-9127-af8e42410423","wAsSubmissionDate":"2024-10-30","wAsAcceptedDate":"2015-09-29","wAsEditorialStatus":"ACCEPTED","wAsBaseArticleType":"Research Article","wAsDisplayArticleType":"Research Article","ibrProduct":{"maId":"JDI","maName":"Journal of Diabetes Investigation","wAsJournalUuid":"f4c16e81-bdcb-4795-9dce-3b36416eb748","wAsNewJournalRevenueModel":"OA","wAsJournalEISSN":"20401124","wAsFlipDate":"2013-09-23","wAsJournalTitle":"Journal of Diabetes Investigation","wAsJournalGroupCode":"JDI","wAsJournalOwnership":null,"wAsJournalStatus":"Yes","wAsEditorialOfficeEmail":"jdi@wiley.com"}}}]}}'}}}</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>20241001203606</t>
+          <t>20241030081442</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>8000029806</t>
+          <t>8000062102</t>
         </is>
       </c>
     </row>
@@ -10373,7 +10366,7 @@
           <t>PaymentType</t>
         </is>
       </c>
-      <c r="E1" s="74" t="inlineStr">
+      <c r="E1" s="73" t="inlineStr">
         <is>
           <t>SalesOrg</t>
         </is>
@@ -10410,118 +10403,118 @@
       </c>
     </row>
     <row r="2" ht="27.5" customHeight="1">
-      <c r="A2" s="78" t="inlineStr">
+      <c r="A2" s="77" t="inlineStr">
         <is>
           <t>Create Order In VIAX</t>
         </is>
       </c>
-      <c r="B2" s="78" t="inlineStr">
+      <c r="B2" s="77" t="inlineStr">
         <is>
           <t>New / Existing</t>
         </is>
       </c>
-      <c r="C2" s="78" t="inlineStr">
+      <c r="C2" s="77" t="inlineStr">
         <is>
           <t>Gold OA</t>
         </is>
       </c>
-      <c r="D2" s="72" t="inlineStr">
+      <c r="D2" s="71" t="inlineStr">
         <is>
           <t>Alipay</t>
         </is>
       </c>
-      <c r="E2" s="72" t="inlineStr">
+      <c r="E2" s="71" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
       </c>
-      <c r="F2" s="72" t="inlineStr">
+      <c r="F2" s="71" t="inlineStr">
         <is>
           <t>Society/Promo/Institutional</t>
         </is>
       </c>
-      <c r="G2" s="72" t="inlineStr">
+      <c r="G2" s="71" t="inlineStr">
         <is>
           <t>China</t>
         </is>
       </c>
-      <c r="H2" s="79" t="n"/>
-      <c r="I2" s="76" t="n">
+      <c r="H2" s="78" t="n"/>
+      <c r="I2" s="75" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="77" t="n"/>
-      <c r="K2" s="77" t="inlineStr">
+      <c r="J2" s="76" t="n"/>
+      <c r="K2" s="76" t="inlineStr">
         <is>
           <t>Create Alipay Order for New Customer with Society discount GOA Order Type</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="73" t="n"/>
-      <c r="B3" s="73" t="n"/>
-      <c r="C3" s="73" t="n"/>
-      <c r="D3" s="73" t="n"/>
-      <c r="E3" s="73" t="n"/>
-      <c r="F3" s="73" t="n"/>
-      <c r="G3" s="73" t="n"/>
+      <c r="A3" s="72" t="n"/>
+      <c r="B3" s="72" t="n"/>
+      <c r="C3" s="72" t="n"/>
+      <c r="D3" s="72" t="n"/>
+      <c r="E3" s="72" t="n"/>
+      <c r="F3" s="72" t="n"/>
+      <c r="G3" s="72" t="n"/>
       <c r="H3" s="49" t="n"/>
-      <c r="I3" s="73" t="n"/>
-      <c r="J3" s="73" t="n"/>
-      <c r="K3" s="73" t="n"/>
+      <c r="I3" s="72" t="n"/>
+      <c r="J3" s="72" t="n"/>
+      <c r="K3" s="72" t="n"/>
     </row>
     <row r="4" ht="12" customHeight="1">
-      <c r="A4" s="73" t="n"/>
-      <c r="B4" s="73" t="n"/>
-      <c r="C4" s="73" t="n"/>
-      <c r="D4" s="73" t="n"/>
-      <c r="E4" s="73" t="n"/>
-      <c r="F4" s="73" t="n"/>
-      <c r="G4" s="73" t="n"/>
+      <c r="A4" s="72" t="n"/>
+      <c r="B4" s="72" t="n"/>
+      <c r="C4" s="72" t="n"/>
+      <c r="D4" s="72" t="n"/>
+      <c r="E4" s="72" t="n"/>
+      <c r="F4" s="72" t="n"/>
+      <c r="G4" s="72" t="n"/>
       <c r="H4" s="49" t="n"/>
-      <c r="I4" s="73" t="n"/>
-      <c r="J4" s="73" t="n"/>
-      <c r="K4" s="73" t="n"/>
+      <c r="I4" s="72" t="n"/>
+      <c r="J4" s="72" t="n"/>
+      <c r="K4" s="72" t="n"/>
     </row>
     <row r="5" hidden="1" ht="14.5" customHeight="1">
-      <c r="A5" s="73" t="n"/>
-      <c r="B5" s="73" t="n"/>
-      <c r="C5" s="73" t="n"/>
-      <c r="D5" s="73" t="n"/>
-      <c r="E5" s="73" t="n"/>
-      <c r="F5" s="73" t="n"/>
-      <c r="G5" s="73" t="n"/>
+      <c r="A5" s="72" t="n"/>
+      <c r="B5" s="72" t="n"/>
+      <c r="C5" s="72" t="n"/>
+      <c r="D5" s="72" t="n"/>
+      <c r="E5" s="72" t="n"/>
+      <c r="F5" s="72" t="n"/>
+      <c r="G5" s="72" t="n"/>
       <c r="H5" s="49" t="inlineStr">
         <is>
           <t>N.A</t>
         </is>
       </c>
-      <c r="I5" s="73" t="n"/>
-      <c r="J5" s="73" t="n"/>
-      <c r="K5" s="73" t="n"/>
+      <c r="I5" s="72" t="n"/>
+      <c r="J5" s="72" t="n"/>
+      <c r="K5" s="72" t="n"/>
     </row>
     <row r="6" hidden="1" ht="19.5" customHeight="1">
-      <c r="A6" s="73" t="n"/>
-      <c r="B6" s="73" t="n"/>
-      <c r="C6" s="73" t="n"/>
-      <c r="D6" s="71" t="n"/>
-      <c r="E6" s="71" t="n"/>
-      <c r="F6" s="71" t="n"/>
-      <c r="G6" s="71" t="n"/>
+      <c r="A6" s="72" t="n"/>
+      <c r="B6" s="72" t="n"/>
+      <c r="C6" s="72" t="n"/>
+      <c r="D6" s="70" t="n"/>
+      <c r="E6" s="70" t="n"/>
+      <c r="F6" s="70" t="n"/>
+      <c r="G6" s="70" t="n"/>
       <c r="H6" s="50" t="n"/>
-      <c r="I6" s="71" t="n"/>
-      <c r="J6" s="71" t="n"/>
-      <c r="K6" s="71" t="n"/>
+      <c r="I6" s="70" t="n"/>
+      <c r="J6" s="70" t="n"/>
+      <c r="K6" s="70" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="73" t="n"/>
-      <c r="B7" s="73" t="n"/>
-      <c r="C7" s="73" t="n"/>
-      <c r="D7" s="75" t="inlineStr">
+      <c r="A7" s="72" t="n"/>
+      <c r="B7" s="72" t="n"/>
+      <c r="C7" s="72" t="n"/>
+      <c r="D7" s="74" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="E7" s="75" t="inlineStr">
+      <c r="E7" s="74" t="inlineStr">
         <is>
           <t>P1</t>
         </is>
@@ -10552,11 +10545,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="73" t="n"/>
-      <c r="B8" s="73" t="n"/>
-      <c r="C8" s="73" t="n"/>
-      <c r="D8" s="73" t="n"/>
-      <c r="E8" s="75" t="inlineStr">
+      <c r="A8" s="72" t="n"/>
+      <c r="B8" s="72" t="n"/>
+      <c r="C8" s="72" t="n"/>
+      <c r="D8" s="72" t="n"/>
+      <c r="E8" s="74" t="inlineStr">
         <is>
           <t>P2</t>
         </is>
@@ -10587,16 +10580,16 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="73" t="n"/>
-      <c r="B9" s="73" t="n"/>
-      <c r="C9" s="73" t="n"/>
-      <c r="D9" s="73" t="n"/>
-      <c r="E9" s="75" t="inlineStr">
+      <c r="A9" s="72" t="n"/>
+      <c r="B9" s="72" t="n"/>
+      <c r="C9" s="72" t="n"/>
+      <c r="D9" s="72" t="n"/>
+      <c r="E9" s="74" t="inlineStr">
         <is>
           <t>P3</t>
         </is>
       </c>
-      <c r="F9" s="75" t="inlineStr">
+      <c r="F9" s="74" t="inlineStr">
         <is>
           <t>Editorial</t>
         </is>
@@ -10622,12 +10615,12 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="73" t="n"/>
-      <c r="B10" s="73" t="n"/>
-      <c r="C10" s="73" t="n"/>
-      <c r="D10" s="73" t="n"/>
-      <c r="E10" s="71" t="n"/>
-      <c r="F10" s="71" t="n"/>
+      <c r="A10" s="72" t="n"/>
+      <c r="B10" s="72" t="n"/>
+      <c r="C10" s="72" t="n"/>
+      <c r="D10" s="72" t="n"/>
+      <c r="E10" s="70" t="n"/>
+      <c r="F10" s="70" t="n"/>
       <c r="G10" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">Germany </t>
@@ -10649,11 +10642,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="73" t="n"/>
-      <c r="B11" s="73" t="n"/>
-      <c r="C11" s="73" t="n"/>
-      <c r="D11" s="73" t="n"/>
-      <c r="E11" s="75" t="inlineStr">
+      <c r="A11" s="72" t="n"/>
+      <c r="B11" s="72" t="n"/>
+      <c r="C11" s="72" t="n"/>
+      <c r="D11" s="72" t="n"/>
+      <c r="E11" s="74" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
@@ -10684,11 +10677,11 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="73" t="n"/>
-      <c r="B12" s="73" t="n"/>
-      <c r="C12" s="73" t="n"/>
-      <c r="D12" s="71" t="n"/>
-      <c r="E12" s="71" t="n"/>
+      <c r="A12" s="72" t="n"/>
+      <c r="B12" s="72" t="n"/>
+      <c r="C12" s="72" t="n"/>
+      <c r="D12" s="70" t="n"/>
+      <c r="E12" s="70" t="n"/>
       <c r="F12" s="52" t="inlineStr">
         <is>
           <t>ArticleType</t>
@@ -10715,15 +10708,15 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="73" t="n"/>
-      <c r="B13" s="73" t="n"/>
-      <c r="C13" s="73" t="n"/>
-      <c r="D13" s="70" t="inlineStr">
+      <c r="A13" s="72" t="n"/>
+      <c r="B13" s="72" t="n"/>
+      <c r="C13" s="72" t="n"/>
+      <c r="D13" s="69" t="inlineStr">
         <is>
           <t>Invoice</t>
         </is>
       </c>
-      <c r="E13" s="70" t="inlineStr">
+      <c r="E13" s="69" t="inlineStr">
         <is>
           <t>P1</t>
         </is>
@@ -10754,11 +10747,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="73" t="n"/>
-      <c r="B14" s="73" t="n"/>
-      <c r="C14" s="73" t="n"/>
-      <c r="D14" s="73" t="n"/>
-      <c r="E14" s="70" t="inlineStr">
+      <c r="A14" s="72" t="n"/>
+      <c r="B14" s="72" t="n"/>
+      <c r="C14" s="72" t="n"/>
+      <c r="D14" s="72" t="n"/>
+      <c r="E14" s="69" t="inlineStr">
         <is>
           <t>P2</t>
         </is>
@@ -10789,16 +10782,16 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="73" t="n"/>
-      <c r="B15" s="73" t="n"/>
-      <c r="C15" s="73" t="n"/>
-      <c r="D15" s="73" t="n"/>
-      <c r="E15" s="70" t="inlineStr">
+      <c r="A15" s="72" t="n"/>
+      <c r="B15" s="72" t="n"/>
+      <c r="C15" s="72" t="n"/>
+      <c r="D15" s="72" t="n"/>
+      <c r="E15" s="69" t="inlineStr">
         <is>
           <t>P3</t>
         </is>
       </c>
-      <c r="F15" s="70" t="inlineStr">
+      <c r="F15" s="69" t="inlineStr">
         <is>
           <t>Editorial</t>
         </is>
@@ -10824,12 +10817,12 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="73" t="n"/>
-      <c r="B16" s="73" t="n"/>
-      <c r="C16" s="73" t="n"/>
-      <c r="D16" s="73" t="n"/>
-      <c r="E16" s="71" t="n"/>
-      <c r="F16" s="71" t="n"/>
+      <c r="A16" s="72" t="n"/>
+      <c r="B16" s="72" t="n"/>
+      <c r="C16" s="72" t="n"/>
+      <c r="D16" s="72" t="n"/>
+      <c r="E16" s="70" t="n"/>
+      <c r="F16" s="70" t="n"/>
       <c r="G16" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">Germany </t>
@@ -10851,11 +10844,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="73" t="n"/>
-      <c r="B17" s="73" t="n"/>
-      <c r="C17" s="73" t="n"/>
-      <c r="D17" s="73" t="n"/>
-      <c r="E17" s="70" t="inlineStr">
+      <c r="A17" s="72" t="n"/>
+      <c r="B17" s="72" t="n"/>
+      <c r="C17" s="72" t="n"/>
+      <c r="D17" s="72" t="n"/>
+      <c r="E17" s="69" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
@@ -10886,11 +10879,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="73" t="n"/>
-      <c r="B18" s="73" t="n"/>
-      <c r="C18" s="73" t="n"/>
-      <c r="D18" s="71" t="n"/>
-      <c r="E18" s="71" t="n"/>
+      <c r="A18" s="72" t="n"/>
+      <c r="B18" s="72" t="n"/>
+      <c r="C18" s="72" t="n"/>
+      <c r="D18" s="70" t="n"/>
+      <c r="E18" s="70" t="n"/>
       <c r="F18" s="55" t="inlineStr">
         <is>
           <t>ArticleType</t>
@@ -10917,15 +10910,15 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="73" t="n"/>
-      <c r="B19" s="73" t="n"/>
-      <c r="C19" s="73" t="n"/>
-      <c r="D19" s="74" t="inlineStr">
+      <c r="A19" s="72" t="n"/>
+      <c r="B19" s="72" t="n"/>
+      <c r="C19" s="72" t="n"/>
+      <c r="D19" s="73" t="inlineStr">
         <is>
           <t>Proforma</t>
         </is>
       </c>
-      <c r="E19" s="74" t="inlineStr">
+      <c r="E19" s="73" t="inlineStr">
         <is>
           <t>P1</t>
         </is>
@@ -10956,11 +10949,11 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="73" t="n"/>
-      <c r="B20" s="73" t="n"/>
-      <c r="C20" s="73" t="n"/>
-      <c r="D20" s="73" t="n"/>
-      <c r="E20" s="74" t="inlineStr">
+      <c r="A20" s="72" t="n"/>
+      <c r="B20" s="72" t="n"/>
+      <c r="C20" s="72" t="n"/>
+      <c r="D20" s="72" t="n"/>
+      <c r="E20" s="73" t="inlineStr">
         <is>
           <t>P2</t>
         </is>
@@ -10991,16 +10984,16 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="73" t="n"/>
-      <c r="B21" s="73" t="n"/>
-      <c r="C21" s="73" t="n"/>
-      <c r="D21" s="73" t="n"/>
-      <c r="E21" s="74" t="inlineStr">
+      <c r="A21" s="72" t="n"/>
+      <c r="B21" s="72" t="n"/>
+      <c r="C21" s="72" t="n"/>
+      <c r="D21" s="72" t="n"/>
+      <c r="E21" s="73" t="inlineStr">
         <is>
           <t>P3</t>
         </is>
       </c>
-      <c r="F21" s="74" t="inlineStr">
+      <c r="F21" s="73" t="inlineStr">
         <is>
           <t>Editorial</t>
         </is>
@@ -11026,12 +11019,12 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="73" t="n"/>
-      <c r="B22" s="73" t="n"/>
-      <c r="C22" s="73" t="n"/>
-      <c r="D22" s="73" t="n"/>
-      <c r="E22" s="71" t="n"/>
-      <c r="F22" s="71" t="n"/>
+      <c r="A22" s="72" t="n"/>
+      <c r="B22" s="72" t="n"/>
+      <c r="C22" s="72" t="n"/>
+      <c r="D22" s="72" t="n"/>
+      <c r="E22" s="70" t="n"/>
+      <c r="F22" s="70" t="n"/>
       <c r="G22" s="45" t="inlineStr">
         <is>
           <t xml:space="preserve">Germany </t>
@@ -11053,11 +11046,11 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="73" t="n"/>
-      <c r="B23" s="73" t="n"/>
-      <c r="C23" s="73" t="n"/>
-      <c r="D23" s="73" t="n"/>
-      <c r="E23" s="74" t="inlineStr">
+      <c r="A23" s="72" t="n"/>
+      <c r="B23" s="72" t="n"/>
+      <c r="C23" s="72" t="n"/>
+      <c r="D23" s="72" t="n"/>
+      <c r="E23" s="73" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
@@ -11088,11 +11081,11 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="71" t="n"/>
-      <c r="B24" s="71" t="n"/>
-      <c r="C24" s="71" t="n"/>
-      <c r="D24" s="71" t="n"/>
-      <c r="E24" s="71" t="n"/>
+      <c r="A24" s="70" t="n"/>
+      <c r="B24" s="70" t="n"/>
+      <c r="C24" s="70" t="n"/>
+      <c r="D24" s="70" t="n"/>
+      <c r="E24" s="70" t="n"/>
       <c r="F24" s="45" t="inlineStr">
         <is>
           <t>ArticleType</t>
@@ -11194,7 +11187,7 @@
           <t>PaymentType</t>
         </is>
       </c>
-      <c r="E1" s="74" t="inlineStr">
+      <c r="E1" s="73" t="inlineStr">
         <is>
           <t>SalesOrg</t>
         </is>
@@ -11226,27 +11219,27 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="78" t="inlineStr">
+      <c r="A2" s="77" t="inlineStr">
         <is>
           <t>Create Order In VIAX</t>
         </is>
       </c>
-      <c r="B2" s="78" t="inlineStr">
+      <c r="B2" s="77" t="inlineStr">
         <is>
           <t>New / Existing</t>
         </is>
       </c>
-      <c r="C2" s="78" t="inlineStr">
+      <c r="C2" s="77" t="inlineStr">
         <is>
           <t>HYBRID OA</t>
         </is>
       </c>
-      <c r="D2" s="72" t="inlineStr">
+      <c r="D2" s="71" t="inlineStr">
         <is>
           <t>Alipay</t>
         </is>
       </c>
-      <c r="E2" s="80" t="inlineStr">
+      <c r="E2" s="79" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
@@ -11256,17 +11249,17 @@
           <t>Society Value</t>
         </is>
       </c>
-      <c r="G2" s="80" t="inlineStr">
+      <c r="G2" s="79" t="inlineStr">
         <is>
           <t>China</t>
         </is>
       </c>
-      <c r="H2" s="76" t="inlineStr">
+      <c r="H2" s="75" t="inlineStr">
         <is>
           <t>N.A</t>
         </is>
       </c>
-      <c r="I2" s="79" t="n">
+      <c r="I2" s="78" t="n">
         <v>0</v>
       </c>
       <c r="J2" s="44" t="inlineStr">
@@ -11276,19 +11269,19 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="73" t="n"/>
-      <c r="B3" s="73" t="n"/>
-      <c r="C3" s="73" t="n"/>
-      <c r="D3" s="71" t="n"/>
-      <c r="E3" s="73" t="n"/>
+      <c r="A3" s="72" t="n"/>
+      <c r="B3" s="72" t="n"/>
+      <c r="C3" s="72" t="n"/>
+      <c r="D3" s="70" t="n"/>
+      <c r="E3" s="72" t="n"/>
       <c r="F3" s="61" t="inlineStr">
         <is>
           <t>Promo %</t>
         </is>
       </c>
-      <c r="G3" s="73" t="n"/>
-      <c r="H3" s="71" t="n"/>
-      <c r="I3" s="73" t="n"/>
+      <c r="G3" s="72" t="n"/>
+      <c r="H3" s="70" t="n"/>
+      <c r="I3" s="72" t="n"/>
       <c r="J3" s="44" t="inlineStr">
         <is>
           <t>Create Order with Promo  Discount (%) P4 with Alipay HOA Order</t>
@@ -11296,15 +11289,15 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="73" t="n"/>
-      <c r="B4" s="73" t="n"/>
-      <c r="C4" s="73" t="n"/>
-      <c r="D4" s="75" t="inlineStr">
+      <c r="A4" s="72" t="n"/>
+      <c r="B4" s="72" t="n"/>
+      <c r="C4" s="72" t="n"/>
+      <c r="D4" s="74" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="E4" s="75" t="inlineStr">
+      <c r="E4" s="74" t="inlineStr">
         <is>
           <t>P1</t>
         </is>
@@ -11334,11 +11327,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="73" t="n"/>
-      <c r="B5" s="73" t="n"/>
-      <c r="C5" s="73" t="n"/>
-      <c r="D5" s="73" t="n"/>
-      <c r="E5" s="75" t="inlineStr">
+      <c r="A5" s="72" t="n"/>
+      <c r="B5" s="72" t="n"/>
+      <c r="C5" s="72" t="n"/>
+      <c r="D5" s="72" t="n"/>
+      <c r="E5" s="74" t="inlineStr">
         <is>
           <t>P2</t>
         </is>
@@ -11368,11 +11361,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="73" t="n"/>
-      <c r="B6" s="73" t="n"/>
-      <c r="C6" s="73" t="n"/>
-      <c r="D6" s="73" t="n"/>
-      <c r="E6" s="75" t="inlineStr">
+      <c r="A6" s="72" t="n"/>
+      <c r="B6" s="72" t="n"/>
+      <c r="C6" s="72" t="n"/>
+      <c r="D6" s="72" t="n"/>
+      <c r="E6" s="74" t="inlineStr">
         <is>
           <t>P3</t>
         </is>
@@ -11402,11 +11395,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="73" t="n"/>
-      <c r="B7" s="73" t="n"/>
-      <c r="C7" s="73" t="n"/>
-      <c r="D7" s="73" t="n"/>
-      <c r="E7" s="71" t="n"/>
+      <c r="A7" s="72" t="n"/>
+      <c r="B7" s="72" t="n"/>
+      <c r="C7" s="72" t="n"/>
+      <c r="D7" s="72" t="n"/>
+      <c r="E7" s="70" t="n"/>
       <c r="F7" s="63" t="inlineStr">
         <is>
           <t>Promo Value</t>
@@ -11432,11 +11425,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="73" t="n"/>
-      <c r="B8" s="73" t="n"/>
-      <c r="C8" s="73" t="n"/>
-      <c r="D8" s="73" t="n"/>
-      <c r="E8" s="75" t="inlineStr">
+      <c r="A8" s="72" t="n"/>
+      <c r="B8" s="72" t="n"/>
+      <c r="C8" s="72" t="n"/>
+      <c r="D8" s="72" t="n"/>
+      <c r="E8" s="74" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
@@ -11466,11 +11459,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="73" t="n"/>
-      <c r="B9" s="73" t="n"/>
-      <c r="C9" s="73" t="n"/>
-      <c r="D9" s="71" t="n"/>
-      <c r="E9" s="71" t="n"/>
+      <c r="A9" s="72" t="n"/>
+      <c r="B9" s="72" t="n"/>
+      <c r="C9" s="72" t="n"/>
+      <c r="D9" s="70" t="n"/>
+      <c r="E9" s="70" t="n"/>
       <c r="F9" s="62" t="inlineStr">
         <is>
           <t>Custom-ZCDA</t>
@@ -11496,15 +11489,15 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="73" t="n"/>
-      <c r="B10" s="73" t="n"/>
-      <c r="C10" s="73" t="n"/>
-      <c r="D10" s="70" t="inlineStr">
+      <c r="A10" s="72" t="n"/>
+      <c r="B10" s="72" t="n"/>
+      <c r="C10" s="72" t="n"/>
+      <c r="D10" s="69" t="inlineStr">
         <is>
           <t>Invoice</t>
         </is>
       </c>
-      <c r="E10" s="70" t="inlineStr">
+      <c r="E10" s="69" t="inlineStr">
         <is>
           <t>P1</t>
         </is>
@@ -11534,11 +11527,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="73" t="n"/>
-      <c r="B11" s="73" t="n"/>
-      <c r="C11" s="73" t="n"/>
-      <c r="D11" s="73" t="n"/>
-      <c r="E11" s="70" t="inlineStr">
+      <c r="A11" s="72" t="n"/>
+      <c r="B11" s="72" t="n"/>
+      <c r="C11" s="72" t="n"/>
+      <c r="D11" s="72" t="n"/>
+      <c r="E11" s="69" t="inlineStr">
         <is>
           <t>P2</t>
         </is>
@@ -11568,11 +11561,11 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="73" t="n"/>
-      <c r="B12" s="73" t="n"/>
-      <c r="C12" s="73" t="n"/>
-      <c r="D12" s="73" t="n"/>
-      <c r="E12" s="70" t="inlineStr">
+      <c r="A12" s="72" t="n"/>
+      <c r="B12" s="72" t="n"/>
+      <c r="C12" s="72" t="n"/>
+      <c r="D12" s="72" t="n"/>
+      <c r="E12" s="69" t="inlineStr">
         <is>
           <t>P3</t>
         </is>
@@ -11602,11 +11595,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="73" t="n"/>
-      <c r="B13" s="73" t="n"/>
-      <c r="C13" s="73" t="n"/>
-      <c r="D13" s="73" t="n"/>
-      <c r="E13" s="71" t="n"/>
+      <c r="A13" s="72" t="n"/>
+      <c r="B13" s="72" t="n"/>
+      <c r="C13" s="72" t="n"/>
+      <c r="D13" s="72" t="n"/>
+      <c r="E13" s="70" t="n"/>
       <c r="F13" s="64" t="inlineStr">
         <is>
           <t>Promo %</t>
@@ -11632,11 +11625,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="73" t="n"/>
-      <c r="B14" s="73" t="n"/>
-      <c r="C14" s="73" t="n"/>
-      <c r="D14" s="73" t="n"/>
-      <c r="E14" s="70" t="inlineStr">
+      <c r="A14" s="72" t="n"/>
+      <c r="B14" s="72" t="n"/>
+      <c r="C14" s="72" t="n"/>
+      <c r="D14" s="72" t="n"/>
+      <c r="E14" s="69" t="inlineStr">
         <is>
           <t>P4</t>
         </is>
@@ -11666,11 +11659,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="71" t="n"/>
-      <c r="B15" s="71" t="n"/>
-      <c r="C15" s="71" t="n"/>
-      <c r="D15" s="71" t="n"/>
-      <c r="E15" s="71" t="n"/>
+      <c r="A15" s="70" t="n"/>
+      <c r="B15" s="70" t="n"/>
+      <c r="C15" s="70" t="n"/>
+      <c r="D15" s="70" t="n"/>
+      <c r="E15" s="70" t="n"/>
       <c r="F15" s="64" t="inlineStr">
         <is>
           <t>Institutional</t>

</xml_diff>